<commit_message>
#14 #32 1124 嗯……
</commit_message>
<xml_diff>
--- a/www/data/flashcard.xlsx
+++ b/www/data/flashcard.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\voc4fun\voc4fun-client\www\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="600" yWindow="30" windowWidth="19395" windowHeight="7845" activeTab="2"/>
   </bookViews>
@@ -4707,11 +4712,11 @@
     <t xml:space="preserve"> [名]青少年;青少年時代                   </t>
   </si>
   <si>
-    <t>中文</t>
+    <t>key</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>英文</t>
+    <t>value</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -4839,6 +4844,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -4886,7 +4894,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4921,7 +4929,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -18156,8 +18164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B786"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A284" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
0315  flashcard delete null
</commit_message>
<xml_diff>
--- a/www/data/flashcard.xlsx
+++ b/www/data/flashcard.xlsx
@@ -1719,8 +1719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+    <sheetView tabSelected="1" topLeftCell="A171" workbookViewId="0">
+      <selection activeCell="A189" sqref="A189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>

</xml_diff>